<commit_message>
Updated a few of the important parts
</commit_message>
<xml_diff>
--- a/Hardware/Parts_List.xlsx
+++ b/Hardware/Parts_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Part</t>
   </si>
@@ -100,12 +100,6 @@
     <t>10k Potentiometer</t>
   </si>
   <si>
-    <t>Processor Power Switch</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/9609</t>
-  </si>
-  <si>
     <t>Ferrite Bead</t>
   </si>
   <si>
@@ -127,9 +121,6 @@
     <t>RJ-45 Jacks</t>
   </si>
   <si>
-    <t>Temp Sensor Connector</t>
-  </si>
-  <si>
     <t>Fan Connectors</t>
   </si>
   <si>
@@ -139,12 +130,6 @@
     <t>Power 2x1 5mm Screw terminals</t>
   </si>
   <si>
-    <t>ATMega Programming Headers</t>
-  </si>
-  <si>
-    <t>LCD Connector</t>
-  </si>
-  <si>
     <t>Ribbon Cable Connector</t>
   </si>
   <si>
@@ -170,6 +155,15 @@
   </si>
   <si>
     <t>http://www.newark.com/texas-instruments/ek-tm4c123gxl/eval-board-tm4c123g-tiva-c-launchpad/dp/73W9275?mckv=jB9TMSt9|pcrid|5184266005|plid|{placement}&amp;CMP=KNC-Y-SKU-MDC</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9806</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/643</t>
+  </si>
+  <si>
+    <t>ATMega Programming Male Headers</t>
   </si>
 </sst>
 </file>
@@ -550,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,13 +577,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -655,7 +649,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -762,6 +756,9 @@
       <c r="B29">
         <v>1</v>
       </c>
+      <c r="C29" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -782,66 +779,66 @@
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="B37">
+        <v>6</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -849,15 +846,15 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -865,33 +862,9 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45">
         <v>1</v>
       </c>
     </row>
@@ -899,11 +872,15 @@
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1"/>
     <hyperlink ref="C9" r:id="rId2"/>
-    <hyperlink ref="C30" r:id="rId3" display="http://www.newark.com/stmicroelectronics/ld1117s33ctr/ic-ldo-volt-reg-3-3v-0-8a-sot/dp/89K0626?CMP=AFC-OP"/>
-    <hyperlink ref="C12" r:id="rId4"/>
-    <hyperlink ref="C34" r:id="rId5"/>
-    <hyperlink ref="C32" r:id="rId6"/>
-    <hyperlink ref="A3" r:id="rId7"/>
+    <hyperlink ref="C12" r:id="rId3"/>
+    <hyperlink ref="C33" r:id="rId4"/>
+    <hyperlink ref="C31" r:id="rId5"/>
+    <hyperlink ref="A3" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C30" r:id="rId8"/>
+    <hyperlink ref="C29" r:id="rId9"/>
+    <hyperlink ref="C34" r:id="rId10"/>
+    <hyperlink ref="C37" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Issue #29 add magnetometer to parts list
</commit_message>
<xml_diff>
--- a/Hardware/Parts_List.xlsx
+++ b/Hardware/Parts_List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Part</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>ATMega Programming Male Headers</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/10530</t>
+  </si>
+  <si>
+    <t>Magnetometer</t>
   </si>
 </sst>
 </file>
@@ -253,6 +259,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -300,7 +309,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -335,7 +344,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -544,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,228 +652,239 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="4">
-        <v>2</v>
-      </c>
-      <c r="C15" s="3"/>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="4">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
       <c r="B23">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29">
         <v>1</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B37">
-        <v>6</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>38</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <v>1</v>
       </c>
     </row>
@@ -872,15 +892,16 @@
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1"/>
     <hyperlink ref="C9" r:id="rId2"/>
-    <hyperlink ref="C12" r:id="rId3"/>
-    <hyperlink ref="C33" r:id="rId4"/>
-    <hyperlink ref="C31" r:id="rId5"/>
+    <hyperlink ref="C13" r:id="rId3"/>
+    <hyperlink ref="C34" r:id="rId4"/>
+    <hyperlink ref="C32" r:id="rId5"/>
     <hyperlink ref="A3" r:id="rId6"/>
     <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C30" r:id="rId8"/>
-    <hyperlink ref="C29" r:id="rId9"/>
-    <hyperlink ref="C34" r:id="rId10"/>
-    <hyperlink ref="C37" r:id="rId11"/>
+    <hyperlink ref="C31" r:id="rId8"/>
+    <hyperlink ref="C30" r:id="rId9"/>
+    <hyperlink ref="C35" r:id="rId10"/>
+    <hyperlink ref="C38" r:id="rId11"/>
+    <hyperlink ref="C12" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Replaced gps diode from
http://www.mouser.com/ProductDetail/Diodes-Incorporated/1N4148WS-7-F/?qs=sGAEpiMZZMtoHjESLttvkr74rFM1mfYSUkQNUJ8i7JM%3d

to

http://www.digikey.com/product-detail/en/CDSW4148-G/641-1459-1-ND/3511544
</commit_message>
<xml_diff>
--- a/Hardware/Parts_List.xlsx
+++ b/Hardware/Parts_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Part</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Green 1206 LED</t>
   </si>
   <si>
-    <t>http://www.mouser.com/ProductDetail/Diodes-Incorporated/1N4148WS-7-F/?qs=sGAEpiMZZMtoHjESLttvkr74rFM1mfYSUkQNUJ8i7JM%3d</t>
-  </si>
-  <si>
     <t>Connectors</t>
   </si>
   <si>
@@ -139,12 +136,6 @@
     <t>http://www.ti.com/tool/ek-tm4c123gxl</t>
   </si>
   <si>
-    <t>Old GPS Diode</t>
-  </si>
-  <si>
-    <t>New Diode</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-detail/en/CDSW4148-G/641-1459-1-ND/3511544</t>
   </si>
   <si>
@@ -164,6 +155,9 @@
   </si>
   <si>
     <t>ATMega Programming Male Headers</t>
+  </si>
+  <si>
+    <t>GPS Diode</t>
   </si>
 </sst>
 </file>
@@ -544,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,13 +571,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -649,7 +643,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -757,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -779,7 +773,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -790,31 +784,34 @@
         <v>1</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" t="s">
         <v>33</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -822,10 +819,7 @@
         <v>34</v>
       </c>
       <c r="B37">
-        <v>6</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -833,7 +827,7 @@
         <v>35</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -841,30 +835,22 @@
         <v>36</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>38</v>
-      </c>
-      <c r="B42">
         <v>1</v>
       </c>
     </row>
@@ -873,14 +859,13 @@
     <hyperlink ref="C7" r:id="rId1"/>
     <hyperlink ref="C9" r:id="rId2"/>
     <hyperlink ref="C12" r:id="rId3"/>
-    <hyperlink ref="C33" r:id="rId4"/>
-    <hyperlink ref="C31" r:id="rId5"/>
-    <hyperlink ref="A3" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C30" r:id="rId8"/>
-    <hyperlink ref="C29" r:id="rId9"/>
-    <hyperlink ref="C34" r:id="rId10"/>
-    <hyperlink ref="C37" r:id="rId11"/>
+    <hyperlink ref="C31" r:id="rId4"/>
+    <hyperlink ref="A3" r:id="rId5"/>
+    <hyperlink ref="C8" r:id="rId6"/>
+    <hyperlink ref="C30" r:id="rId7"/>
+    <hyperlink ref="C29" r:id="rId8"/>
+    <hyperlink ref="C33" r:id="rId9"/>
+    <hyperlink ref="C36" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the ferrite bead in BOM
</commit_message>
<xml_diff>
--- a/Hardware/Parts_List.xlsx
+++ b/Hardware/Parts_List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -103,9 +103,6 @@
     <t>Ferrite Bead</t>
   </si>
   <si>
-    <t>http://www.newark.com/wurth-elektronik/742792701/ferrite-bead-0-05ohm-500ma-0402/dp/78R5663</t>
-  </si>
-  <si>
     <t>Red 1206 LED</t>
   </si>
   <si>
@@ -170,6 +167,9 @@
   </si>
   <si>
     <t>Magnetometer</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/vishay-dale/ilbb0603er100v/ferrite-bead-0-05ohm-500ma-0603/dp/53K5027</t>
   </si>
 </sst>
 </file>
@@ -309,7 +309,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -344,7 +344,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -555,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C31" sqref="A28:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,13 +586,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -652,13 +652,13 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -669,7 +669,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -777,7 +777,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -788,69 +788,69 @@
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38">
         <v>6</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -858,7 +858,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -866,7 +866,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41">
         <v>2</v>
@@ -874,7 +874,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -882,7 +882,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -897,11 +897,10 @@
     <hyperlink ref="C32" r:id="rId5"/>
     <hyperlink ref="A3" r:id="rId6"/>
     <hyperlink ref="C8" r:id="rId7"/>
-    <hyperlink ref="C31" r:id="rId8"/>
-    <hyperlink ref="C30" r:id="rId9"/>
-    <hyperlink ref="C35" r:id="rId10"/>
-    <hyperlink ref="C38" r:id="rId11"/>
-    <hyperlink ref="C12" r:id="rId12"/>
+    <hyperlink ref="C30" r:id="rId8"/>
+    <hyperlink ref="C35" r:id="rId9"/>
+    <hyperlink ref="C38" r:id="rId10"/>
+    <hyperlink ref="C12" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
#77 Updated Parts List for IMU
</commit_message>
<xml_diff>
--- a/Hardware/Parts_List.xlsx
+++ b/Hardware/Parts_List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Part</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Ribbon Cable Connector</t>
   </si>
   <si>
-    <t>http://www.adafruit.com/products/790</t>
-  </si>
-  <si>
     <t>http://www.ti.com/tool/ek-tm4c123gxl</t>
   </si>
   <si>
@@ -158,6 +155,15 @@
   </si>
   <si>
     <t>http://www.newark.com/vishay-dale/ilbb0603er100v/ferrite-bead-0-05ohm-500ma-0603/dp/53K5027</t>
+  </si>
+  <si>
+    <t>IMU</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/STMicroelectronics/INEMO-M1/?qs=sGAEpiMZZMtE0my147CO44HKeQPfxWIC</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/CIB10P100NC/1276-6388-1-ND/3973917</t>
   </si>
 </sst>
 </file>
@@ -224,7 +230,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -236,6 +242,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -246,6 +255,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -294,7 +306,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -329,7 +341,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -538,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,13 +583,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -643,142 +655,142 @@
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="4">
-        <v>2</v>
-      </c>
-      <c r="C15" s="3"/>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="4">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
       <c r="B23">
-        <v>36</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29">
         <v>1</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -788,8 +800,8 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>46</v>
+      <c r="A33" t="s">
+        <v>30</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -798,59 +810,70 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36">
-        <v>6</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>36</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>1</v>
       </c>
     </row>
@@ -859,14 +882,16 @@
     <hyperlink ref="C7" r:id="rId1"/>
     <hyperlink ref="C9" r:id="rId2"/>
     <hyperlink ref="C12" r:id="rId3"/>
-    <hyperlink ref="C31" r:id="rId4"/>
+    <hyperlink ref="C32" r:id="rId4"/>
     <hyperlink ref="A3" r:id="rId5"/>
     <hyperlink ref="C8" r:id="rId6"/>
-    <hyperlink ref="C30" r:id="rId7"/>
-    <hyperlink ref="C29" r:id="rId8"/>
-    <hyperlink ref="C33" r:id="rId9"/>
-    <hyperlink ref="C36" r:id="rId10"/>
+    <hyperlink ref="C31" r:id="rId7"/>
+    <hyperlink ref="C30" r:id="rId8"/>
+    <hyperlink ref="C34" r:id="rId9"/>
+    <hyperlink ref="C37" r:id="rId10"/>
+    <hyperlink ref="C13" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated parts list with new processor
</commit_message>
<xml_diff>
--- a/Hardware/Parts_List.xlsx
+++ b/Hardware/Parts_List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Part</t>
   </si>
@@ -64,9 +64,6 @@
     <t>22pF</t>
   </si>
   <si>
-    <t>100nF</t>
-  </si>
-  <si>
     <t>0.1uF</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>16 mhZ Crystal</t>
   </si>
   <si>
-    <t>10k Potentiometer</t>
-  </si>
-  <si>
     <t>Ferrite Bead</t>
   </si>
   <si>
@@ -124,9 +118,6 @@
     <t>Power 2x1 5mm Screw terminals</t>
   </si>
   <si>
-    <t>Ribbon Cable Connector</t>
-  </si>
-  <si>
     <t>http://www.ti.com/tool/ek-tm4c123gxl</t>
   </si>
   <si>
@@ -139,12 +130,6 @@
     <t>http://www.mouser.com/ProductDetail/OSRAM-Opto-Semiconductors/LH-N974-KN-1/?qs=sGAEpiMZZMt82OzCyDsLFAV097Vn80XJzM0DIFS2How%3d</t>
   </si>
   <si>
-    <t>http://www.newark.com/texas-instruments/ek-tm4c123gxl/eval-board-tm4c123g-tiva-c-launchpad/dp/73W9275?mckv=jB9TMSt9|pcrid|5184266005|plid|{placement}&amp;CMP=KNC-Y-SKU-MDC</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/9806</t>
-  </si>
-  <si>
     <t>https://www.sparkfun.com/products/643</t>
   </si>
   <si>
@@ -163,7 +148,55 @@
     <t>http://www.mouser.com/ProductDetail/STMicroelectronics/INEMO-M1/?qs=sGAEpiMZZMtE0my147CO44HKeQPfxWIC</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-detail/en/CIB10P100NC/1276-6388-1-ND/3973917</t>
+    <t>http://www.adafruit.com/products/790</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/kemet/c1206c220j5gactu/capacitor-ceramic-22pf-50v-c0g/dp/70K9304</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/multicomp/mc1206b104k500ct/capacitor-ceramic-0-1uf-50v-x7r/dp/06R4208</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/avx/12065c105kat2a/capacitor-ceramic-1uf-50v-x7r/dp/10R6014</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/taiyo-yuden/gmk316f106zl-t/capacitor-ceramic-10uf-35v-y5v/dp/30K5465</t>
+  </si>
+  <si>
+    <t>http://www.ti.com/tool/ek-tm4c1294xl#buy</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/multicomp/mc0125w12061330r/resistor-330r-0-125w-1-1206/dp/94W6668</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/multicomp/mchp06w2f1200t5e/resistor-high-power-120-ohm-500mw/dp/01N7140</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/vishay-dale/crcw12061k00fkea/resistor-thick-film-1kohm-250mw/dp/53K1779?MER=PPSO_N_P_EverywhereElse_None</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/vishay-dale/crcw120610k0fkea/resistor-thick-film-10kohm-250mw/dp/53K1907?MER=PPSO_N_P_EverywhereElse_None</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9144</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/8432</t>
+  </si>
+  <si>
+    <t>http://www.newark.com/harting/60-05-068-5100/socket-scsi-pcb-straight-68w/dp/21M4933?ost=Harting+60+05+068+5100</t>
+  </si>
+  <si>
+    <t>Ribbon Cable Male Connector</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/536</t>
+  </si>
+  <si>
+    <t>Magnetometer</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/10530</t>
   </si>
 </sst>
 </file>
@@ -217,7 +250,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -225,12 +258,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -244,6 +292,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -306,7 +357,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,7 +392,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -550,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,13 +634,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -655,243 +706,282 @@
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4">
+        <v>2</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>30</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="7" t="s">
+    </row>
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4">
-        <v>2</v>
-      </c>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>21</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>22</v>
       </c>
       <c r="B24">
         <v>36</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26">
         <v>3</v>
       </c>
+      <c r="C26" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29">
         <v>1</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>30</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37">
-        <v>6</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
+      <c r="C41" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1"/>
     <hyperlink ref="C9" r:id="rId2"/>
-    <hyperlink ref="C12" r:id="rId3"/>
-    <hyperlink ref="C32" r:id="rId4"/>
-    <hyperlink ref="A3" r:id="rId5"/>
-    <hyperlink ref="C8" r:id="rId6"/>
-    <hyperlink ref="C31" r:id="rId7"/>
-    <hyperlink ref="C30" r:id="rId8"/>
-    <hyperlink ref="C34" r:id="rId9"/>
-    <hyperlink ref="C37" r:id="rId10"/>
-    <hyperlink ref="C13" r:id="rId11"/>
+    <hyperlink ref="C31" r:id="rId3"/>
+    <hyperlink ref="A3" r:id="rId4"/>
+    <hyperlink ref="C8" r:id="rId5"/>
+    <hyperlink ref="C30" r:id="rId6"/>
+    <hyperlink ref="C33" r:id="rId7"/>
+    <hyperlink ref="C36" r:id="rId8"/>
+    <hyperlink ref="C13" r:id="rId9"/>
+    <hyperlink ref="C12" r:id="rId10" display="//www.google.com/url?q=http%3A%2F%2Fwww.adafruit.com%2Fproducts%2F790"/>
+    <hyperlink ref="C17" r:id="rId11" display="//www.google.com/url?q=http%3A%2F%2Fwww.newark.com%2Fkemet%2Fc1206c220j5gactu%2Fcapacitor-ceramic-22pf-50v-c0g%2Fdp%2F70K9304"/>
+    <hyperlink ref="C18" r:id="rId12" display="//www.google.com/url?q=http%3A%2F%2Fwww.newark.com%2Fmulticomp%2Fmc1206b104k500ct%2Fcapacitor-ceramic-0-1uf-50v-x7r%2Fdp%2F06R4208"/>
+    <hyperlink ref="C19" r:id="rId13" display="//www.google.com/url?q=http%3A%2F%2Fwww.newark.com%2Favx%2F12065c105kat2a%2Fcapacitor-ceramic-1uf-50v-x7r%2Fdp%2F10R6014"/>
+    <hyperlink ref="C20" r:id="rId14" display="//www.google.com/url?q=http%3A%2F%2Fwww.newark.com%2Ftaiyo-yuden%2Fgmk316f106zl-t%2Fcapacitor-ceramic-10uf-35v-y5v%2Fdp%2F30K5465"/>
+    <hyperlink ref="C23" r:id="rId15" display="//www.google.com/url?q=http%3A%2F%2Fwww.newark.com%2Fmulticomp%2Fmc0125w12061330r%2Fresistor-330r-0-125w-1-1206%2Fdp%2F94W6668"/>
+    <hyperlink ref="C24" r:id="rId16" display="//www.google.com/url?q=http%3A%2F%2Fwww.newark.com%2Fmulticomp%2Fmchp06w2f1200t5e%2Fresistor-high-power-120-ohm-500mw%2Fdp%2F01N7140"/>
+    <hyperlink ref="C25" r:id="rId17" display="//www.google.com/url?q=http%3A%2F%2Fwww.newark.com%2Fvishay-dale%2Fcrcw12061k00fkea%2Fresistor-thick-film-1kohm-250mw%2Fdp%2F53K1779%3FMER%3DPPSO_N_P_EverywhereElse_None"/>
+    <hyperlink ref="C26" r:id="rId18" display="//www.google.com/url?q=http%3A%2F%2Fwww.newark.com%2Fvishay-dale%2Fcrcw120610k0fkea%2Fresistor-thick-film-10kohm-250mw%2Fdp%2F53K1907%3FMER%3DPPSO_N_P_EverywhereElse_None"/>
+    <hyperlink ref="C38" r:id="rId19" display="//www.google.com/url?q=https%3A%2F%2Fwww.sparkfun.com%2Fproducts%2F9144"/>
+    <hyperlink ref="C39" r:id="rId20" display="//www.google.com/url?q=https%3A%2F%2Fwww.sparkfun.com%2Fproducts%2F8432"/>
+    <hyperlink ref="C41" r:id="rId21" display="//www.google.com/url?q=http%3A%2F%2Fwww.newark.com%2Fharting%2F60-05-068-5100%2Fsocket-scsi-pcb-straight-68w%2Fdp%2F21M4933%3Fost%3DHarting%2B60%2B05%2B068%2B5100"/>
+    <hyperlink ref="C29" r:id="rId22" display="//www.google.com/url?q=https%3A%2F%2Fwww.sparkfun.com%2Fproducts%2F536"/>
+    <hyperlink ref="C14" r:id="rId23" display="//www.google.com/url?q=https%3A%2F%2Fwww.sparkfun.com%2Fproducts%2F10530"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>